<commit_message>
R code for generating document-term matrix. Almost done
</commit_message>
<xml_diff>
--- a/skills210322.xlsx
+++ b/skills210322.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d52fed4db2de6dc/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d52fed4db2de6dc/Documents/academic/CUNY SPS/DATA 607/Proj3/zachsfr project three/Data-607-Project-Three/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{F46F01D4-20E3-4571-93DE-9B04C42D761D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E9F5D085-EFE8-4642-8E38-11B795A14A43}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{F46F01D4-20E3-4571-93DE-9B04C42D761D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC050C2A-FB08-4B4C-A6BB-E23CEE619ABF}"/>
   <bookViews>
-    <workbookView xWindow="19092" yWindow="3768" windowWidth="23040" windowHeight="12204" xr2:uid="{78AA6224-A4A1-46E6-8D4A-7F5081C4FAD3}"/>
+    <workbookView xWindow="7680" yWindow="3768" windowWidth="23040" windowHeight="12204" xr2:uid="{78AA6224-A4A1-46E6-8D4A-7F5081C4FAD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>analysis</t>
   </si>
@@ -190,6 +190,39 @@
   </si>
   <si>
     <t>cassandra</t>
+  </si>
+  <si>
+    <t>csharp</t>
+  </si>
+  <si>
+    <t>cplusplus</t>
+  </si>
+  <si>
+    <t>computerscience</t>
+  </si>
+  <si>
+    <t>dataengineering</t>
+  </si>
+  <si>
+    <t>deeplearning</t>
+  </si>
+  <si>
+    <t>machinelearning</t>
+  </si>
+  <si>
+    <t>neuralnetworks</t>
+  </si>
+  <si>
+    <t>projectmanagement</t>
+  </si>
+  <si>
+    <t>scikitlearn</t>
+  </si>
+  <si>
+    <t>softwaredevelopment</t>
+  </si>
+  <si>
+    <t>softwareengineering</t>
   </si>
 </sst>
 </file>
@@ -541,279 +574,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A07168-52AF-4505-BF9F-CE86C29232B1}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:A41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C52">
     <sortCondition ref="A1:A52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>